<commit_message>
Updated Phyiscs 1, project 1
</commit_message>
<xml_diff>
--- a/Feeney's assignment schedule.xlsx
+++ b/Feeney's assignment schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543BCC0A-CD71-4E1C-A93A-81AA9483FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3804F1F5-CA25-4EC4-9401-57C22E4E2DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="1680" windowWidth="19155" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="2" r:id="rId1"/>
@@ -736,20 +736,20 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1796875" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -812,7 +812,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -860,7 +860,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -869,16 +869,16 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -894,7 +894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -920,7 +920,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -962,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -996,16 +996,16 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="3.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1040,7 +1040,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1049,7 +1049,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Worked on the sprite PNG to PLY cube model thing as well as edited some of the Defender sprites
</commit_message>
<xml_diff>
--- a/Feeney's assignment schedule.xlsx
+++ b/Feeney's assignment schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3804F1F5-CA25-4EC4-9401-57C22E4E2DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3753314E-1B8C-4E25-A74A-F44BE3A9DB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="2" r:id="rId1"/>
@@ -733,23 +733,23 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -788,7 +788,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -812,7 +812,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -860,7 +860,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -878,7 +878,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -894,7 +894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -920,7 +920,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -962,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -996,16 +996,16 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1040,7 +1040,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1049,7 +1049,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -1122,7 +1122,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Push that should have happend on Wednesday
</commit_message>
<xml_diff>
--- a/Feeney's assignment schedule.xlsx
+++ b/Feeney's assignment schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E44512-070D-48FB-B81B-7AD918348F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E148AA3-1CC1-4D74-B94A-CF13055A806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="2" r:id="rId1"/>
@@ -562,16 +562,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -857,23 +857,23 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,11 +884,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -924,7 +924,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -936,7 +936,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -948,7 +948,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="27.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1010,17 +1010,17 @@
         <v>26</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1028,15 +1028,15 @@
         <v>27</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1062,7 +1062,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1074,7 +1074,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1126,16 +1126,16 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1188,38 +1188,38 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>4</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>5</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>6</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -1252,29 +1252,29 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>10</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>11</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Start of broad phase AABB grid speed up
</commit_message>
<xml_diff>
--- a/Feeney's assignment schedule.xlsx
+++ b/Feeney's assignment schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E148AA3-1CC1-4D74-B94A-CF13055A806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F45410-AAC6-454D-9AE7-1C99DA52F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>INFO-6044</t>
   </si>
@@ -452,13 +452,19 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Project #2 (Nov. 29th)</t>
+  </si>
+  <si>
+    <t>Project #3 (Due: Dec. 7th)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +499,14 @@
     <font>
       <strike/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -543,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,6 +586,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -860,7 +877,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12:F12"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1045,7 +1062,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="7"/>
@@ -1071,7 +1088,9 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
@@ -1086,7 +1105,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Added static lua .lib file
</commit_message>
<xml_diff>
--- a/Feeney's assignment schedule.xlsx
+++ b/Feeney's assignment schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F45410-AAC6-454D-9AE7-1C99DA52F3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79533B7D-B2A5-48B2-8EE8-3EC311C13791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actual" sheetId="2" r:id="rId1"/>
@@ -582,13 +582,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -873,24 +873,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B87C30-35AF-4600-80F3-443B5D985714}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="D16:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.26953125" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,11 +901,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -917,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -929,7 +929,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -941,7 +941,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -989,7 +989,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="27.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1062,12 +1062,12 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1145,16 +1145,16 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="3.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" customWidth="1"/>
-    <col min="6" max="6" width="23.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1207,38 +1207,38 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>5</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>6</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>7</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>8</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>9</v>
       </c>
@@ -1271,29 +1271,29 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>10</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>11</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1302,7 +1302,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>